<commit_message>
it finally works on the apple netflix and cvs earnings the problem was that \s encompases newlines and tabs as well as normal space I had to just use a literal space character in the regex
</commit_message>
<xml_diff>
--- a/data/output.xlsx
+++ b/data/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>person</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -446,22 +446,12 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>comapny</t>
+          <t>type</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
           <t>text</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>ender</t>
         </is>
       </c>
     </row>
@@ -471,35 +461,28 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>QUESTION AND ANSWER SECTION
-Jessica Reif Ehrlich</t>
+          <t>Erik W. Woodring</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, Morgan Stanley &amp; Co. LLC</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Thank you. Well, let's start with the topic du jour; not one but two strikes. Can you give us your views of how this
-affects your business on a practical basis? How far out does your original content take you? And how much of the
-content spend do you think gets pushed from this year into next year?</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Hey. Good afternoon, guys. Thank you so much for taking the questions. Tim, maybe if we start with you, if we go
+back to the December quarter and the production shutdowns around that time, I think the question a lot of us were
+asking was how should we think about the deferral of demand versus destruction of demand. March quarter was
+quite strong, 2% year-over-year iPhone growth. And so, as we sit here in May, how have you seen that customers
+that weren't able to purchase during the December quarter behave, meaning are you seeing that they deferred
+purchases to March and June? Could they be deferring purchases to later in hopes of buying a new iPhone? Just
+how should maybe we think about the cadence of that? And then, I have a follow-up. Thanks.</t>
         </is>
       </c>
     </row>
@@ -509,33 +492,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Erik W. Woodring</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, Morgan Stanley &amp; Co. LLC</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>In terms of the content, how much original content do you have? Do you run out like at a certain point in time, you
-probably will.</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Okay, perfect. Thank you for that color. And Tim, maybe to follow up, it's been three or four quarters now that
+you've mentioned emerging markets like India and others. And I imagine having just opened two new stores in the
+country, it's clearly an important market for you. So, maybe can you just talk about why you see India as such an
+important market and others, how you think about monetization trends in the country, and specifically, what you
+have to do within the country to really ensure that India becomes maybe a more material mix of your business?
+And that's it for me. Thanks so much.</t>
         </is>
       </c>
     </row>
@@ -545,34 +522,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Erik W. Woodring</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, Morgan Stanley &amp; Co. LLC</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Absolutely. So let's move on to password sharing, which is something everyone on the call wants to hear about.
-Could you give us kind of like state of the union? What progress have you made to-date? And when will the rollout
-be complete?</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Thank you so much.</t>
         </is>
       </c>
     </row>
@@ -582,35 +547,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Michael Ng</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, Goldman Sachs &amp; Co. LLC</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Is there a way to think about segments of borrowers who have yet to convert? It feels like there's another wave
-coming or maybe several waves, maybe college students who are home for the summer and will go back in
-August or September. I don't know that mobile devices have been shut off yet. Anecdotally, many people who are
-not on mobile devices have said they haven't been cut off yet. So can you help us think through that?</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Hey. Good afternoon. Thank you very much for the question. It was encouraging to hear about the record
+installed base across iPhone and across all devices. It's been, I think, double-digit growth over the last few years
+across the active devices. I was just wondering, is that a good way to think about the installed base growth going
+forward? And then, for the iPhone installed base specifically, I was just wondering if you could provide a little bit of
+texture around how you think about the growth there whether regionally or by first smartphones versus switchers.
+And then, I have a quick follow-up.</t>
         </is>
       </c>
     </row>
@@ -620,34 +577,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Michael Ng</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, Goldman Sachs &amp; Co. LLC</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Can you provide any color on the results? Like, what percent have converted to paying and on what plan? Like,
-[indiscernible] (00:06:08) members versus subscribers? Your subscriber numbers were great this quarter, but
-they were also add-ons to households. So can you help us think through? And did people change plans?</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Great. Excellent. And then, it was also encouraging to see the number of devices per iPhone user continuing to
+grow. I was just wondering if you could talk about the opportunity to continue to increase that number of Apple
+devices per iPhone user, and if you have any color around how the monetization per user may differ from those,
+for lack of a better word, super-users versus those that may not be as deep into the ecosystem. Thanks.</t>
         </is>
       </c>
     </row>
@@ -657,34 +605,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Michael Ng</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, Goldman Sachs &amp; Co. LLC</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Well, maybe if you can help us think through like, in UCAN, how much of the ARM growth is a function of add-on
-members to existing accounts versus new subs signing up to higher-priced plans. And it sounds like from your
-letter that ARM will accelerate in second half as you get further along in password sharings. Is that correct?</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Excellent. Thank you, Tim.</t>
         </is>
       </c>
     </row>
@@ -694,39 +630,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Wamsi Mohan</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, BofA Securities, Inc.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>But there's another surprise that you had in the last couple of weeks, which seems like it could also be a very
-positive driver to ARM, and that is that you dropped the basic plan in Canada several weeks ago, and you just
-announced that in the US and UK. So I guess a couple of questions here.
-Are there any plans for the rest of the world? And has it so far, from your experience in Canada, has it driven the
-response that you hoped for? Is the response that more people go to the advertising tier? And then, I guess, one
-other final part of this question is that it's an obvious positive for ARPU. It feels like the impact is like $5 or more
-per month. When this is fully rolled out over three years or so â€“ like, over what period of time do you think this will
-have the most impact?</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Yes. Thank you. Tim, you had called out on December quarter earnings that Pro models were significantly
+constrained. Did you see a catch-up on the Pro models specifically in the March quarter and was the mix better
+than typical? And do you see that mix renormalizing here in the June quarter and maybe you can comment on the
+channel inventory levels as well for iPhones? And I have a follow-up.</t>
         </is>
       </c>
     </row>
@@ -736,33 +658,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Wamsi Mohan</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, BofA Securities, Inc.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>So, one last question and then I'll move on to advertising. But, for your new members or new subs from the
-password sharing, are there any noticeable differences in churn?</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Okay. Thanks, Tim. And Tim, as a follow-up, you've launched so many services around Apple Pay. Most recently,
+you mentioned buy now, pay later, a high-yield savings account. Where do you see the expansion in the
+payments ecosystem over time? And do you look at the payments ecosystem as a standalone revenue
+opportunity or is it more about making the devices even more inseparable from us? Thank you.</t>
         </is>
       </c>
     </row>
@@ -772,32 +686,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Wamsi Mohan</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, BofA Securities, Inc.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Right.</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Thanks, Tim.</t>
         </is>
       </c>
     </row>
@@ -807,35 +711,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>David Vogt</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, UBS Securities LLC</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Moving on to advertising, could you give me some color on some of the innovative or nontraditional offerings that
-you have? One of the things you talked about in the upfront was like offering advertisers the ability to go into the
-top 10, which is it provides an incredible reach; that guaranteed reach really all the time. Could you just talk
-through some of the ways because you're thinking in ways that are very different from traditional media.</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Great. Thanks for taking my question. Tim, I just wanted to go back to maybe kind of dig into the restocking of
+inventory in the channel versus what we're hearing from a demand perspective that appears to be a little bit softer
+in the March quarter from some of your larger carriers that exhibited relatively weak upgrade rates. So, just want
+to kind of get a sense for where you're seeing demand signals today vis-Ã -vis how you were thinking about it
+maybe a month ago or even three months ago. And is there sort of an acceleration in demand or any sort of
+signals that you might want to share with us at this point? And then, I have a follow-up.</t>
         </is>
       </c>
     </row>
@@ -845,33 +741,27 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>David Vogt</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, UBS Securities LLC</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Has there been any change to advertising ARM since last quarter when you said advertising ARM was at least as
-high as the standard tier, indicating that advertising only part of it was $8.50 or more?</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Great. That's helpful. And then, just quickly on services, are you seeing anything in terms of consumers' behavior
+other than sort of the macro that you mentioned and tough comps on digital advertising and mobile gaming? Are
+you seeing users of all the disparate services change in what they're using and how they're using it and time
+spent with an Apple service, now that we're technically hopefully fully past COVID with China almost fully
+reopened? I'm just trying to get a sense for how user or consumer behaviors changed over the last three to six
+months. Thanks.</t>
         </is>
       </c>
     </row>
@@ -881,34 +771,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>David Vogt</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, UBS Securities LLC</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Can you tell us about your initial up-front advertising performance? You seem to have everything advertisers are
-looking for, but this is a really tepid overall advertising environment. So is there anything you can say about what
-the reaction's been?</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Great. Thanks, guys.</t>
         </is>
       </c>
     </row>
@@ -918,32 +796,28 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Samik Chatterjee</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, JPMorgan Securities LLC</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>What tools and how much time do you need to like invest to build your own ad tech infrastructure?</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Yeah. Hi. Thanks for taking my questions. I guess maybe I can follow up on David's question here on services.
+And in the past, pre-pandemic, the growth rate there was more about sort of mid-teens. The growth rates today
+where you stand, even if I back out FX impact, is more about low double-digits. So, one of the questions that we
+get often from investors and want to get your thoughts on is, even as the installed base growth seems to have
+accelerated, are these more cyclical drivers that are depressing growth at this point from returning to that level or
+do you see more of a roll-out on the monetization that you need to do to get back to those growth levels? And I
+have a follow-up, please.</t>
         </is>
       </c>
     </row>
@@ -953,33 +827,28 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Samik Chatterjee</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, JPMorgan Securities LLC</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Is there like a time period? Like, in order to achieve scale, is this like a three-year plan before you feel like you
-really have all the tech capabilities in place?</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Okay. And maybe if I can just follow up, this is more of a macro question. I don't know if, Luca, you or Tim want to
+take this. But obviously, the macro is not sort of helpful at this point. But what you're sort of implying in terms of
+your guide is momentum for your products remains pretty stable. You're actually guiding to a modest uptick ex FX
+for the overall business. I mean, what are you seeing in terms of customer sort of spending trends, and overall,
+does the consumer sort of continue to deteriorate in terms of spending patterns? And is your sort of momentum
+here just a function of share gains? How should we think about sort of where the consumer is versus what your
+products are doing independent of that?</t>
         </is>
       </c>
     </row>
@@ -989,34 +858,22 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Samik Chatterjee</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, JPMorgan Securities LLC</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Spence, this one may be for you, but what's your vision for the advertising contribution? You've said in the past
-that you like it to be 10% of revenue. But, given the decline of linear, are you rethinking this so that it would be a
-higher percent?</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Thank you. Thanks for taking my questions.</t>
         </is>
       </c>
     </row>
@@ -1026,34 +883,37 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Amit Daryanani</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, Evercore ISI</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Sure. But maybe to follow-up on what you just said, like, where do you think the pool of ad dollars will come from
-over time? Given all the capabilities that Greg just talked about, why would it be limited to linear? Because you're
-going to have such extraordinary capabilities. Shouldn't the pool be linear and digital?</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>I have two as well. I guess first off on gross margins for the June quarter, they seem to be holding up fairly well,
+especially given the fact that sales are going down on a sequential basis. So, Luca, I'm wondering if you can just
+touch on what's driving the strength in gross margin sequentially that's offsetting the lack of leverage, if you may.
+And then, I also notice that the range of your gross margin guide is 50 basis points. It's typically 100 basis points.
+What does that entail? What does that mean?
+Luca Maestri
+Chief Financial Officer &amp; Senior Vice President, Apple, Inc.                                                                                                                                                                                               A
+So, you're right. I mean, we are guiding to a fairly stable level of gross margins at a very high level. We're very
+happy with the gross margins that we're having this cycle. For the first time in several quarters, we expect foreign
+exchange to be flat on a sequential basis at the gross margin level. Unfortunately, still a headwind at the revenue
+level. But at gross margin level, sequentially, we expect foreign exchange not to be a factor. And so, the seasonal
+loss of leverage that you're referring to, we expect to be offset by cost savings. And so, that should give us that
+level of margins. As you know â€“ you were asking about 50 basis points. We have guided to 50 basis points of a
+range before as well. This year in particular, because of the 14th week in the â€“ during the December quarter,
+we're a bit late in the calendar year, right. And so, we have a bit more visibility around margins for the June
+quarter.</t>
         </is>
       </c>
     </row>
@@ -1063,33 +923,24 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Amit Daryanani</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, Evercore ISI</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>One last question on this and then I'll move on. But has engagement changed in the past quarter or so? Are there
-any noticeable differences between the tiers?</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Got it. That's helpful. And then, I guess, Tim, if I just kind of go back to the India discussion a bit, perhaps you
+could just contrast what you're seeing in India today versus what you saw in China maybe a decade or so ago. Is
+that a reasonable ramp to think India would have or could it be different from the lessons you've seen in China?</t>
         </is>
       </c>
     </row>
@@ -1099,34 +950,22 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Amit Daryanani</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, Evercore ISI</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>So let's move on to free cash flow. You had an extraordinary quarter this second quarter, and you talked about
-the outlook for Q3. Could you just maybe address the underlying dynamics, talk a little bit about content spend
-and other investments?</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Thank you.</t>
         </is>
       </c>
     </row>
@@ -1136,32 +975,26 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Krish Sankar</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, TD Cowen</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>What's the content spend outlook for the next few years? What is normal post the strikes, plural?</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Yeah. Hi. Thanks for taking my question. The first question I had is for Tim. Tim, you have primarily been a
+consumer-centric company. But it seems like the line is blurring with the iPhone, iPad, hardware products being
+used for corporate applications. So, is there a way to segment how much of your revenues today are coming from
+enterprise versus consumer? And does the slower corporate IT spend impact your outlook for iPhone, iPad, Mac,
+et cetera? And then, I had a follow-up.</t>
         </is>
       </c>
     </row>
@@ -1171,34 +1004,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Krish Sankar</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, TD Cowen</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>But with your content spend very measured, let's put it that way, and you're kind of maybe investing in ad tech
-capabilities. But, beyond that, like it feel like there's tremendous leverage in your business model. So is there a
-way to think about growth in free cash flow beyond 2024?</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Got it, Tim. Thanks for that. And then, just as a follow-up, obviously, lot of questions on the India retail opening.
+I'm just kind of curious, you also mentioned that you hope to convert a lot of folks into iPhone there. Where do you
+think the biggest opportunity is? Is it like primarily a hardware business like the iPhone, iPad, Wearables, et
+cetera? Or do you think there is a service opportunity in India longer term too? Thank you very much.</t>
         </is>
       </c>
     </row>
@@ -1208,33 +1032,22 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Krish Sankar</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, TD Cowen</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>So can we talk about uses of free cash flow and maybe possibly M&amp;A? There are a lot of distressed assets in
-media land, maybe the lowest multiples in memory that we've seen. What assets might be interesting to you?</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Thanks a lot, Tim.</t>
         </is>
       </c>
     </row>
@@ -1244,34 +1057,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Aaron Rakers</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, Wells Fargo Securities LLC</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>And just maybe moving a little bit away from that, but you've developed a library over 10-plus years at this point.
-And it's pretty substantial, and you've got some really amazing global titles. Would you consider selling your
-library content to others?</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Yeah. Thanks for taking the questions. I guess my first question is, I want to go back to kind of the geographical
+dynamics. I'm curious, as we all think about the reopening attributes of China, just how you would characterize the
+shaping of demand you saw through the course of this last quarter and kind of how you're thinking about the
+impact of that reopening playing out over the next couple quarters?</t>
         </is>
       </c>
     </row>
@@ -1281,32 +1085,26 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Aaron Rakers</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, Wells Fargo Securities LLC</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>And do you</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Yeah. Very helpful, Tim. As a quick follow-up, I want to go back to Amit's question on gross margin. You talked
+about FX, the lessening impact there. I'm just curious of when you look at our gross margin, obviously, you got
+mix attributes kind of potentially continuing to drive that higher. But I'm curious on the current environment how
+you would characterize the component pricing dynamics and what you're thinking about in this current quarter's
+guidance.</t>
         </is>
       </c>
     </row>
@@ -1316,32 +1114,22 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Aaron Rakers</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, Wells Fargo Securities LLC</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Oh my God. Okay. Well, and then</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Thank you.</t>
         </is>
       </c>
     </row>
@@ -1351,32 +1139,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Sidney Ho</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, Deutsche Bank Securities, Inc.</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Okay. Well, can you talk a little bit about your live strategy including sports experimentation?</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Great. Thanks for taking my question. I was hoping we can talk about the linearity of the March quarter and
+perhaps the first 4.5 weeks of the current quarter. It looks like things are slowing down quite a bit elsewhere. But if
+my math is right, your fiscal third quarter guidance implies product revenue will be a little bit lower than seasonal
+average on a sequential basis. Any color would be helpful. Thanks.</t>
         </is>
       </c>
     </row>
@@ -1386,33 +1167,130 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Jessica Reif Ehrlich</t>
+          <t>Sidney Ho</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Analyst, Deutsche Bank Securities, Inc.</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>BofA Securities, Inc.</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>There seems to be a lot going on in sports. You supposedly outbid or reportedly outbid ESPN for NFL sports
-documentary. So maybe if you can include in live sports that would be great.</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>EndOfBlock</t>
+          <t>Okay. That's helpful. Maybe as a quick follow-up, you talked about Apple Pay Later. How has the feedback been
+so far and how do you expect the adoption of that service over the next few quarters? Thank you.</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Sidney Ho</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Analyst, Deutsche Bank Securities, Inc.</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Q</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Okay. Thank you.</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Harsh V. Kumar</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Analyst, Piper Sandler &amp; Co.</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Q</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Yeah. Hey, guys. Thanks for squeezing me in. Tim, you're one of the largest chip companies. You're not a
+component maker. You actually use your own products. But we almost never hear in any context of you guys
+being a beneficiary â€“ Apple being a beneficiary for either the CHIPS Act money or the R&amp;D tax credit that's being
+proposed. I was just curious if you're eligible for any of those. And then, I've got a follow-up.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Harsh V. Kumar</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Analyst, Piper Sandler &amp; Co.</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Q</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Understood, and thanks for the clarification. And Luca, I wanted to clarify your comments about June. When
+you're saying June performance will be similar to March, I assume on a year-on-year basis, which would be June
+should be down about 2-something-odd-percent. Is that a fair way? And then, my question that I wanted to ask â€“
+maybe another one for Tim was where do you think is the largest opportunity in your services offering? I mean,
+you're doing a great job. You just set a record, but surely there must be areas where you think you can do better.</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Harsh V. Kumar</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Analyst, Piper Sandler &amp; Co.</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Q</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Understood. Thanks, Tim.</t>
         </is>
       </c>
     </row>

</xml_diff>